<commit_message>
remove configs from file
</commit_message>
<xml_diff>
--- a/startIntegrationAPIRun/configs.xlsx
+++ b/startIntegrationAPIRun/configs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlieemple/local-workspace/MTA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlieemple/cse-workspace/scripts/startIntegrationAPIRun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C2041-51F7-914F-B766-A293E31C1E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C8C53D-EC5B-DC47-A744-15FDC5B917BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17000" xr2:uid="{54811A27-C6E6-9045-909A-299BE06FFB8C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>connectorType</t>
   </si>
@@ -53,31 +53,10 @@
     <t>processingDirection</t>
   </si>
   <si>
-    <t>List all Business Capabilities</t>
-  </si>
-  <si>
-    <t>list_all_business_capabilities</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>952144a8-3730-482d-86f6-eac3133687ef</t>
-  </si>
-  <si>
-    <t>outbound</t>
-  </si>
-  <si>
     <t>processingMode</t>
   </si>
   <si>
-    <t>partial</t>
-  </si>
-  <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
   </si>
 </sst>
 </file>
@@ -429,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0D0FB7-2A45-154E-9BD6-5553C95FBEC9}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,33 +444,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>